<commit_message>
feat: Implement comprehensive solar calculator with Results dashboard
- Added Results route to main.tsx with routing configuration
- Enhanced ProductManagement.tsx with better PV module handling
- Updated main.ts with correct port priority (5174 first)
- Enhanced preload.ts with additional IPC handlers
- Updated solar_calculator_bridge.py with professional PV modules
- Added comprehensive calculation PDF specification
- Updated database with new product data
- Added test files for PV modules and database validation

Features:
- Professional solar calculation engine
- German formatting and localization
- KPI dashboard with technical metrics
- Energy flow analysis
- Economic analysis (NPV, IRR, LCOE)
- CO2 environmental impact calculations
- Battery storage integration
- Export and print functionality
</commit_message>
<xml_diff>
--- a/data/Produkte.xlsx
+++ b/data/Produkte.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\Desktop\Kakerlake 1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF3140E-E23E-4328-B5FC-44386EA706EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFC9A5A-0120-473E-A807-AD1E57082523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$V$142</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="224">
   <si>
     <t xml:space="preserve">Vitovolt 300-DG M440HC </t>
   </si>
@@ -341,30 +344,9 @@
     <t>Tierabwehrschutz</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -437,63 +419,6 @@
     <t>updated_at</t>
   </si>
   <si>
-    <t>kategorie</t>
-  </si>
-  <si>
-    <t>hersteller</t>
-  </si>
-  <si>
-    <t>preis_stück</t>
-  </si>
-  <si>
-    <t>pv_modul_leistung</t>
-  </si>
-  <si>
-    <t>produkt_modell</t>
-  </si>
-  <si>
-    <t>kapazitaet_speicher_kwh</t>
-  </si>
-  <si>
-    <t>wr_leistung_kw</t>
-  </si>
-  <si>
-    <t>ladezyklen_speicher</t>
-  </si>
-  <si>
-    <t>garantie_zeit</t>
-  </si>
-  <si>
-    <t>mass_laenge</t>
-  </si>
-  <si>
-    <t>mass_breite</t>
-  </si>
-  <si>
-    <t>mass_gewicht_kg</t>
-  </si>
-  <si>
-    <t>wirkungsgrad_prozent</t>
-  </si>
-  <si>
-    <t>hersteller_land</t>
-  </si>
-  <si>
-    <t>beschreibung_info</t>
-  </si>
-  <si>
-    <t>eigenschaft_info</t>
-  </si>
-  <si>
-    <t>spezial_merkmal</t>
-  </si>
-  <si>
-    <t>rating_null_zehn</t>
-  </si>
-  <si>
-    <t>PV Modul</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vitovolt 300-DG M470HC </t>
   </si>
   <si>
@@ -729,6 +654,63 @@
   </si>
   <si>
     <t xml:space="preserve">ECS4100 -H2 8,06 kWh </t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>price_euro</t>
+  </si>
+  <si>
+    <t>capacity_w</t>
+  </si>
+  <si>
+    <t>storage_power_kw</t>
+  </si>
+  <si>
+    <t>power_kw</t>
+  </si>
+  <si>
+    <t>max_cycles</t>
+  </si>
+  <si>
+    <t>warranty_years</t>
+  </si>
+  <si>
+    <t>length_m</t>
+  </si>
+  <si>
+    <t>width_m</t>
+  </si>
+  <si>
+    <t>weight_kg</t>
+  </si>
+  <si>
+    <t>efficiency_percent</t>
+  </si>
+  <si>
+    <t>origin_country</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>pros</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>modul</t>
   </si>
 </sst>
 </file>
@@ -815,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -847,12 +829,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1137,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -1166,72 +1147,72 @@
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>131</v>
+    <row r="1" spans="1:26" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="Z1" s="10"/>
     </row>
@@ -1240,7 +1221,7 @@
         <v>1144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
@@ -1249,7 +1230,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F2" s="8">
         <v>440</v>
@@ -1309,7 +1290,7 @@
         <v>1145</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>1</v>
@@ -1318,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>71</v>
@@ -1378,7 +1359,7 @@
         <v>1146</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>2</v>
@@ -1387,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F4" s="8">
         <v>450</v>
@@ -1447,7 +1428,7 @@
         <v>1147</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>3</v>
@@ -1516,7 +1497,7 @@
         <v>1148</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
@@ -1525,7 +1506,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F6" s="8">
         <v>460</v>
@@ -1585,10 +1566,10 @@
         <v>1284</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -1654,10 +1635,10 @@
         <v>1285</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
@@ -1723,7 +1704,7 @@
         <v>1149</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
@@ -1732,7 +1713,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F9" s="8">
         <v>440</v>
@@ -1792,7 +1773,7 @@
         <v>1150</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
@@ -1801,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F10" s="8">
         <v>445</v>
@@ -1861,7 +1842,7 @@
         <v>1151</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1870,7 +1851,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F11" s="8">
         <v>450</v>
@@ -1930,7 +1911,7 @@
         <v>1152</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>12</v>
@@ -1999,7 +1980,7 @@
         <v>1153</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>13</v>
@@ -2008,7 +1989,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F13" s="8">
         <v>460</v>
@@ -2068,10 +2049,10 @@
         <v>1278</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>6</v>
@@ -2137,10 +2118,10 @@
         <v>1279</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>6</v>
@@ -2206,7 +2187,7 @@
         <v>1154</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>14</v>
@@ -2215,7 +2196,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F16" s="8">
         <v>440</v>
@@ -2275,7 +2256,7 @@
         <v>1155</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>15</v>
@@ -2284,7 +2265,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F17" s="8">
         <v>445</v>
@@ -2344,7 +2325,7 @@
         <v>1156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>16</v>
@@ -2353,7 +2334,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F18" s="8">
         <v>450</v>
@@ -2413,7 +2394,7 @@
         <v>1157</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>17</v>
@@ -2482,7 +2463,7 @@
         <v>1158</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>18</v>
@@ -2491,7 +2472,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F20" s="8">
         <v>460</v>
@@ -2551,10 +2532,10 @@
         <v>1280</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>7</v>
@@ -2620,10 +2601,10 @@
         <v>1281</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>7</v>
@@ -2689,16 +2670,16 @@
         <v>1159</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F23" s="8">
         <v>440</v>
@@ -2758,16 +2739,16 @@
         <v>1160</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F24" s="8">
         <v>445</v>
@@ -2827,16 +2808,16 @@
         <v>1161</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F25" s="8">
         <v>450</v>
@@ -2896,10 +2877,10 @@
         <v>1162</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>8</v>
@@ -2965,16 +2946,16 @@
         <v>1163</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F27" s="8">
         <v>460</v>
@@ -3034,10 +3015,10 @@
         <v>1282</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>8</v>
@@ -3103,10 +3084,10 @@
         <v>1283</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>8</v>
@@ -3175,13 +3156,13 @@
         <v>19</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>70</v>
@@ -3244,13 +3225,13 @@
         <v>19</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>70</v>
@@ -3313,7 +3294,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>25</v>
@@ -3382,7 +3363,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>25</v>
@@ -3451,7 +3432,7 @@
         <v>19</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>25</v>
@@ -3520,7 +3501,7 @@
         <v>19</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>25</v>
@@ -3589,7 +3570,7 @@
         <v>19</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>26</v>
@@ -3658,7 +3639,7 @@
         <v>19</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>21</v>
@@ -3727,7 +3708,7 @@
         <v>19</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>21</v>
@@ -3796,7 +3777,7 @@
         <v>19</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>21</v>
@@ -3865,7 +3846,7 @@
         <v>19</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>21</v>
@@ -3934,7 +3915,7 @@
         <v>19</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>21</v>
@@ -4003,7 +3984,7 @@
         <v>19</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>21</v>
@@ -4072,13 +4053,13 @@
         <v>19</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>70</v>
@@ -4141,13 +4122,13 @@
         <v>19</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>70</v>
@@ -4210,13 +4191,13 @@
         <v>19</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>70</v>
@@ -4279,13 +4260,13 @@
         <v>19</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>70</v>
@@ -4348,13 +4329,13 @@
         <v>19</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>70</v>
@@ -4417,7 +4398,7 @@
         <v>19</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>22</v>
@@ -4486,7 +4467,7 @@
         <v>19</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>22</v>
@@ -4555,7 +4536,7 @@
         <v>19</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>22</v>
@@ -4624,7 +4605,7 @@
         <v>19</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>22</v>
@@ -4693,13 +4674,13 @@
         <v>19</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>70</v>
@@ -4762,7 +4743,7 @@
         <v>19</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>20</v>
@@ -4831,13 +4812,13 @@
         <v>19</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>70</v>
@@ -4900,13 +4881,13 @@
         <v>19</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>70</v>
@@ -4969,13 +4950,13 @@
         <v>19</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>70</v>
@@ -5038,7 +5019,7 @@
         <v>19</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>20</v>
@@ -5107,7 +5088,7 @@
         <v>19</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>20</v>
@@ -5176,7 +5157,7 @@
         <v>19</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>20</v>
@@ -5245,7 +5226,7 @@
         <v>19</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>20</v>
@@ -5314,13 +5295,13 @@
         <v>19</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>70</v>
@@ -5383,13 +5364,13 @@
         <v>19</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>70</v>
@@ -5452,13 +5433,13 @@
         <v>19</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>70</v>
@@ -5521,7 +5502,7 @@
         <v>34</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>23</v>
@@ -5529,8 +5510,8 @@
       <c r="E64" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F64" s="7">
-        <v>5.0999999999999996</v>
+      <c r="F64" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G64" s="7">
         <v>5.0999999999999996</v>
@@ -5590,7 +5571,7 @@
         <v>34</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>23</v>
@@ -5598,8 +5579,8 @@
       <c r="E65" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F65" s="7">
-        <v>10.199999999999999</v>
+      <c r="F65" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G65" s="7">
         <v>10.199999999999999</v>
@@ -5659,7 +5640,7 @@
         <v>34</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>23</v>
@@ -5667,8 +5648,8 @@
       <c r="E66" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F66" s="7">
-        <v>15.3</v>
+      <c r="F66" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G66" s="7">
         <v>15.3</v>
@@ -5728,7 +5709,7 @@
         <v>34</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>28</v>
@@ -5736,8 +5717,8 @@
       <c r="E67" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F67" s="7">
-        <v>8.06</v>
+      <c r="F67" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G67" s="7">
         <v>8.06</v>
@@ -5797,7 +5778,7 @@
         <v>34</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>28</v>
@@ -5805,8 +5786,8 @@
       <c r="E68" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F68" s="7">
-        <v>12.09</v>
+      <c r="F68" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G68" s="7">
         <v>12.09</v>
@@ -5866,7 +5847,7 @@
         <v>34</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>28</v>
@@ -5874,8 +5855,8 @@
       <c r="E69" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F69" s="7">
-        <v>16.12</v>
+      <c r="F69" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G69" s="7">
         <v>16.12</v>
@@ -5935,7 +5916,7 @@
         <v>34</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>28</v>
@@ -5943,8 +5924,8 @@
       <c r="E70" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F70" s="7">
-        <v>20.149999999999999</v>
+      <c r="F70" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G70" s="7">
         <v>20.149999999999999</v>
@@ -6004,7 +5985,7 @@
         <v>34</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>28</v>
@@ -6012,8 +5993,8 @@
       <c r="E71" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F71" s="7">
-        <v>24.18</v>
+      <c r="F71" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G71" s="7">
         <v>24.18</v>
@@ -6073,7 +6054,7 @@
         <v>34</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>28</v>
@@ -6081,8 +6062,8 @@
       <c r="E72" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F72" s="7">
-        <v>28.21</v>
+      <c r="F72" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G72" s="7">
         <v>28.21</v>
@@ -6150,8 +6131,8 @@
       <c r="E73" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F73" s="8">
-        <v>3.65</v>
+      <c r="F73" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G73" s="8">
         <v>3.65</v>
@@ -6219,8 +6200,8 @@
       <c r="E74" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F74" s="8">
-        <v>7.3</v>
+      <c r="F74" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G74" s="8">
         <v>7.3</v>
@@ -6288,8 +6269,8 @@
       <c r="E75" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F75" s="8">
-        <v>10.9</v>
+      <c r="F75" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G75" s="8">
         <v>10.9</v>
@@ -6357,8 +6338,8 @@
       <c r="E76" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F76" s="8">
-        <v>14.6</v>
+      <c r="F76" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G76" s="8">
         <v>14.6</v>
@@ -6426,8 +6407,8 @@
       <c r="E77" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F77" s="8">
-        <v>18.25</v>
+      <c r="F77" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G77" s="8">
         <v>18.25</v>
@@ -6495,8 +6476,8 @@
       <c r="E78" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F78" s="8">
-        <v>21.9</v>
+      <c r="F78" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G78" s="8">
         <v>21.9</v>
@@ -6556,7 +6537,7 @@
         <v>34</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>30</v>
@@ -6564,8 +6545,8 @@
       <c r="E79" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F79" s="7">
-        <v>6.6</v>
+      <c r="F79" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G79" s="7">
         <v>6.6</v>
@@ -6625,7 +6606,7 @@
         <v>34</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>30</v>
@@ -6633,8 +6614,8 @@
       <c r="E80" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F80" s="7">
-        <v>9.9</v>
+      <c r="F80" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G80" s="7">
         <v>9.9</v>
@@ -6694,7 +6675,7 @@
         <v>34</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>30</v>
@@ -6702,8 +6683,8 @@
       <c r="E81" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F81" s="7">
-        <v>13.2</v>
+      <c r="F81" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G81" s="7">
         <v>13.2</v>
@@ -6763,7 +6744,7 @@
         <v>34</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>30</v>
@@ -6771,8 +6752,8 @@
       <c r="E82" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F82" s="7">
-        <v>16.399999999999999</v>
+      <c r="F82" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G82" s="7">
         <v>16.399999999999999</v>
@@ -6840,8 +6821,8 @@
       <c r="E83" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F83" s="8">
-        <v>60</v>
+      <c r="F83" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G83" s="8">
         <v>60</v>
@@ -6901,7 +6882,7 @@
         <v>34</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>31</v>
@@ -6909,8 +6890,8 @@
       <c r="E84" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F84" s="7">
-        <v>5</v>
+      <c r="F84" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G84" s="7">
         <v>5</v>
@@ -6970,7 +6951,7 @@
         <v>34</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>31</v>
@@ -6978,8 +6959,8 @@
       <c r="E85" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F85" s="7">
-        <v>10</v>
+      <c r="F85" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G85" s="7">
         <v>10</v>
@@ -7039,7 +7020,7 @@
         <v>34</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>31</v>
@@ -7047,8 +7028,8 @@
       <c r="E86" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F86" s="7">
-        <v>15</v>
+      <c r="F86" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G86" s="7">
         <v>15</v>
@@ -7108,7 +7089,7 @@
         <v>34</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>31</v>
@@ -7116,8 +7097,8 @@
       <c r="E87" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F87" s="7">
-        <v>20</v>
+      <c r="F87" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G87" s="7">
         <v>20</v>
@@ -7177,7 +7158,7 @@
         <v>34</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>31</v>
@@ -7185,8 +7166,8 @@
       <c r="E88" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F88" s="7">
-        <v>25</v>
+      <c r="F88" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G88" s="7">
         <v>25</v>
@@ -7246,7 +7227,7 @@
         <v>34</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>31</v>
@@ -7254,8 +7235,8 @@
       <c r="E89" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F89" s="7">
-        <v>30</v>
+      <c r="F89" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G89" s="7">
         <v>30</v>
@@ -7315,7 +7296,7 @@
         <v>34</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>31</v>
@@ -7323,8 +7304,8 @@
       <c r="E90" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F90" s="7">
-        <v>7</v>
+      <c r="F90" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G90" s="7">
         <v>7</v>
@@ -7384,7 +7365,7 @@
         <v>34</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>31</v>
@@ -7392,8 +7373,8 @@
       <c r="E91" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F91" s="7">
-        <v>14</v>
+      <c r="F91" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G91" s="7">
         <v>14</v>
@@ -7453,7 +7434,7 @@
         <v>34</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>31</v>
@@ -7461,8 +7442,8 @@
       <c r="E92" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F92" s="7">
-        <v>21</v>
+      <c r="F92" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G92" s="7">
         <v>21</v>
@@ -7522,7 +7503,7 @@
         <v>34</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>32</v>
@@ -7530,8 +7511,8 @@
       <c r="E93" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F93" s="7">
-        <v>10</v>
+      <c r="F93" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G93" s="7">
         <v>10</v>
@@ -7591,7 +7572,7 @@
         <v>34</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>32</v>
@@ -7599,8 +7580,8 @@
       <c r="E94" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F94" s="7">
-        <v>15</v>
+      <c r="F94" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G94" s="7">
         <v>15</v>
@@ -7660,7 +7641,7 @@
         <v>34</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>32</v>
@@ -7668,8 +7649,8 @@
       <c r="E95" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F95" s="7">
-        <v>20</v>
+      <c r="F95" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G95" s="7">
         <v>20</v>
@@ -7729,7 +7710,7 @@
         <v>34</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>32</v>
@@ -7737,8 +7718,8 @@
       <c r="E96" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F96" s="7">
-        <v>25</v>
+      <c r="F96" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G96" s="7">
         <v>25</v>
@@ -7798,7 +7779,7 @@
         <v>34</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>32</v>
@@ -7806,8 +7787,8 @@
       <c r="E97" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F97" s="7">
-        <v>30</v>
+      <c r="F97" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G97" s="7">
         <v>30</v>
@@ -7867,7 +7848,7 @@
         <v>34</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>32</v>
@@ -7875,8 +7856,8 @@
       <c r="E98" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F98" s="7">
-        <v>35</v>
+      <c r="F98" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G98" s="7">
         <v>35</v>
@@ -7936,7 +7917,7 @@
         <v>34</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>32</v>
@@ -7944,8 +7925,8 @@
       <c r="E99" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F99" s="7">
-        <v>40</v>
+      <c r="F99" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G99" s="7">
         <v>40</v>
@@ -8005,7 +7986,7 @@
         <v>34</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>33</v>
@@ -8013,8 +7994,8 @@
       <c r="E100" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F100" s="7">
-        <v>5</v>
+      <c r="F100" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G100" s="7">
         <v>5</v>
@@ -8074,7 +8055,7 @@
         <v>34</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>33</v>
@@ -8082,8 +8063,8 @@
       <c r="E101" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F101" s="7">
-        <v>10</v>
+      <c r="F101" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="G101" s="7">
         <v>10</v>
@@ -8143,7 +8124,7 @@
         <v>34</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>33</v>
@@ -8151,8 +8132,8 @@
       <c r="E102" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F102" s="7">
-        <v>15</v>
+      <c r="F102" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G102" s="7">
         <v>15</v>
@@ -9934,7 +9915,7 @@
         <v>1262</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>66</v>
@@ -10003,7 +9984,7 @@
         <v>1263</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>67</v>
@@ -10072,7 +10053,7 @@
         <v>1264</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>68</v>
@@ -10219,16 +10200,16 @@
         <v>92</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="H132" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I132" s="8">
         <v>0</v>
@@ -10287,16 +10268,16 @@
         <v>92</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="H133" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I133" s="8">
         <v>0</v>
@@ -10355,16 +10336,16 @@
         <v>92</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="H134" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I134" s="8">
         <v>0</v>
@@ -10423,16 +10404,16 @@
         <v>92</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G135" s="7" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="H135" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I135" s="8">
         <v>0</v>
@@ -10491,16 +10472,16 @@
         <v>92</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="H136" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I136" s="8">
         <v>0</v>
@@ -10559,16 +10540,16 @@
         <v>92</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F137" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="H137" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I137" s="8">
         <v>0</v>
@@ -10627,16 +10608,16 @@
         <v>92</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="H138" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I138" s="8">
         <v>0</v>
@@ -10695,16 +10676,16 @@
         <v>92</v>
       </c>
       <c r="E139" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="H139" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I139" s="8">
         <v>0</v>
@@ -10763,16 +10744,16 @@
         <v>92</v>
       </c>
       <c r="E140" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F140" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F140" s="7" t="s">
-        <v>126</v>
-      </c>
       <c r="G140" s="7" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="H140" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I140" s="8">
         <v>0</v>
@@ -10831,16 +10812,16 @@
         <v>92</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H141" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I141" s="8">
         <v>0</v>
@@ -10899,16 +10880,16 @@
         <v>92</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H142" s="8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I142" s="8">
         <v>0</v>
@@ -12022,6 +12003,7 @@
       <c r="F330" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V142" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>